<commit_message>
TMTC0019257_VerifyContactsValidationRulesAndWorkFlows - 18 July 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0019257_VerifyContactsValidationRulesAndWorkFlows.xlsx
+++ b/TestData/TMTC0019257_VerifyContactsValidationRulesAndWorkFlows.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D478A50-F49B-436B-B7D0-11234A6C6E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9F3BEE-18FE-4A6E-817D-F8E6CD56E8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
-    <sheet name="RecentlyViewedListView" sheetId="5" r:id="rId2"/>
+    <sheet name="AdditionalInfo" sheetId="5" r:id="rId2"/>
     <sheet name="Contact" sheetId="4" r:id="rId3"/>
-    <sheet name="ExternalContactTabs" sheetId="6" r:id="rId4"/>
-    <sheet name="ExternalContactSections" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Users</t>
   </si>
@@ -64,63 +62,6 @@
     <t>testLVContact@email.com</t>
   </si>
   <si>
-    <t>ListViewValues</t>
-  </si>
-  <si>
-    <t>All Contacts</t>
-  </si>
-  <si>
-    <t>External Contact List</t>
-  </si>
-  <si>
-    <t>HL Employee</t>
-  </si>
-  <si>
-    <t>Modified This Week</t>
-  </si>
-  <si>
-    <t>New This Week</t>
-  </si>
-  <si>
-    <t>Recently Viewed Contacts</t>
-  </si>
-  <si>
-    <t>Recently Viewed</t>
-  </si>
-  <si>
-    <t>TabNames</t>
-  </si>
-  <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>Relationships</t>
-  </si>
-  <si>
-    <t>Coverage</t>
-  </si>
-  <si>
-    <t>Activity</t>
-  </si>
-  <si>
-    <t>Campaign History</t>
-  </si>
-  <si>
-    <t>History</t>
-  </si>
-  <si>
-    <t>Flag Contact</t>
-  </si>
-  <si>
-    <t>Company Details</t>
-  </si>
-  <si>
-    <t>SectionNames</t>
-  </si>
-  <si>
-    <t>PDC Sample</t>
-  </si>
-  <si>
     <t>Admin User</t>
   </si>
   <si>
@@ -128,6 +69,21 @@
   </si>
   <si>
     <t>Amanda Donovan</t>
+  </si>
+  <si>
+    <t>Assistant Name</t>
+  </si>
+  <si>
+    <t>Assistant Phone</t>
+  </si>
+  <si>
+    <t>Assistant Email</t>
+  </si>
+  <si>
+    <t>Test Assistant</t>
+  </si>
+  <si>
+    <t>assistant@email.com</t>
   </si>
 </sst>
 </file>
@@ -468,7 +424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -482,15 +438,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -501,65 +457,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238E81D2-2BA2-4C65-87A5-507061E9159C}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{D7CAAABC-A859-4619-8EC4-97D36FC3B166}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -568,7 +506,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,89 +558,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB32D73B-F2F0-43BC-B4A3-CB0797846C81}">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48A305A-A37C-40D9-9C23-6BCDEA070B36}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes - 19 July
</commit_message>
<xml_diff>
--- a/TestData/TMTC0019257_VerifyContactsValidationRulesAndWorkFlows.xlsx
+++ b/TestData/TMTC0019257_VerifyContactsValidationRulesAndWorkFlows.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCC8255-9CB5-4D34-8B59-63EF83529F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FC63FA-9637-46E4-A988-CFD172D0862B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="AdditionalInfo" sheetId="5" r:id="rId2"/>
     <sheet name="Contact" sheetId="4" r:id="rId3"/>
-    <sheet name="SubscriptionPreferences" sheetId="6" r:id="rId4"/>
+    <sheet name="EventBadges" sheetId="7" r:id="rId4"/>
+    <sheet name="SubscriptionPreferences" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Users</t>
   </si>
@@ -115,6 +116,12 @@
   </si>
   <si>
     <t>Insights/Content</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
   </si>
 </sst>
 </file>
@@ -604,11 +611,48 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B68B1A-37EE-4B14-8A8E-11AB1A6F3387}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF34E67-58AC-465A-81FD-DACA29404DC1}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>